<commit_message>
validation on sales page
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,295 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ordered date</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Payment Method</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Order Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>32</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2022-10-12 10:31:27.779051+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>94890</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>24</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2022-10-05 16:12:12.889207+00:00</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>39999</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>33</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2022-10-12 10:32:43.152822+00:00</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>79999</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>34</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2022-10-12 10:38:56.212365+00:00</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>39999</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>26</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>sivasai</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2022-10-06 04:59:29.405285+00:00</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>109999</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Shipped</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>38</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2022-10-12 12:00:28.772960+00:00</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>39999</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>36</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2022-10-12 11:01:09.182136+00:00</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>49999</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>35</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ajmal11</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2022-10-12 10:39:16.264868+00:00</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>109999</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Cash On Deivery</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Cancelled</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update on guestuser and offers
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,1504 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ordered date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Payment Method</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Order Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>71</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:34:37.993185+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>39999</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>53</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:22:41.891272+00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>369996</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>54</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:37:32.108993+00:00</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>72</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:40:46.492229+00:00</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>49999</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>55</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:43:49.002476+00:00</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>56</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:53:04.659210+00:00</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>73</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:42:16.824941+00:00</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>57</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:54:59.485714+00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2022-10-14 04:58:03.122201+00:00</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>75</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:47:06.091157+00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>159998</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>32</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2022-10-12 10:31:27.779051+00:00</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>95</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>safdar</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2022-10-22 07:29:02.932590+00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>49999</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Out of Delivery</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>24</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2022-10-05 16:12:12.889207+00:00</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>39999</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>33</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2022-10-12 10:32:43.152822+00:00</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>34</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2022-10-12 10:38:56.212365+00:00</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>39999</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>26</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sivasai</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2022-10-06 04:59:29.405285+00:00</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Shipped</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>77</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:52:03.287055+00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>159998</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>103</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2022-10-25 08:19:33.401302+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>108999</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>38</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2022-10-12 12:00:28.772960+00:00</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>39999</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>36</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2022-10-12 11:01:09.182136+00:00</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>49999</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>79</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2022-10-20 06:57:14.322651+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>35</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ajmal11</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2022-10-12 10:39:16.264868+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>94</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2022-10-22 03:40:56.229665+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>79499</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Return Accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>81</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2022-10-20 07:02:16.784814+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>82</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2022-10-20 07:04:10.852020+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>39999</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>60</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2022-10-17 11:06:13.227510+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>189997</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>63</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2022-10-19 07:10:59.408122+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>1099990</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>64</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2022-10-19 08:05:23.043202+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>92</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2022-10-21 09:45:30.537797+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>49999</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>23</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2021-10-05 13:11:54.885994+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Cash On Deivery</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>84</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2022-10-21 04:51:47.715390+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>219998</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>85</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2022-10-21 05:42:24.159709+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>86</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2022-10-21 05:59:17.404048+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>87</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2022-10-21 06:01:58.021945+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>49999</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Order Confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>102</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2022-10-24 05:53:46.660623+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>108899</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>104</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2022-10-25 09:43:45.399500+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>109999</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Out of Delivery</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>88</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2022-10-21 06:08:17.181592+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>79999</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ordered</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>91</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2022-10-21 06:20:24.321775+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>109499</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Return Rejected</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>90</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2022-10-21 06:16:59.991471+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>94390</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Return Accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>83</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2022-10-20 07:05:11.341127+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>159998</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ordered</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>89</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2022-10-21 06:13:56.252845+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>94890</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Shipped</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>101</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2022-10-23 10:14:43.991520+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>153998.1</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Return Accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>100</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2022-10-23 10:13:37.011056+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>124998.1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Razorpay</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Return Accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>93</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2022-10-21 09:46:21.205586+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>79499</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Return Accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>99</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2022-10-23 10:10:49.694471+00:00</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>188998</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>98</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2022-10-23 10:01:11.053683+00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>268997</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>96</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>shameemmm</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2022-10-23 09:55:33.944572+00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>392887</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Cash on Delivery</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>